<commit_message>
format socket stream as per configuration
</commit_message>
<xml_diff>
--- a/app/uploads/GMAT.xlsx
+++ b/app/uploads/GMAT.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>timestamp</t>
   </si>
@@ -50,9 +50,6 @@
     <t>notes</t>
   </si>
   <si>
-    <t>seconds from a reference Julian date</t>
-  </si>
-  <si>
     <t>vx</t>
   </si>
   <si>
@@ -138,12 +135,30 @@
   </si>
   <si>
     <t>warn_low</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>datatype</t>
+  </si>
+  <si>
+    <t>Julian date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -205,9 +220,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -523,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -537,45 +552,48 @@
     <col min="4" max="4" width="9.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" customWidth="1"/>
     <col min="10" max="10" width="31.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -583,33 +601,36 @@
         <v>2</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>2415020.5</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1000000000000</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1E+16</v>
+        <v>2444239.5</v>
+      </c>
+      <c r="G2" s="4">
+        <v>2469807.5</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2524593.5</v>
       </c>
       <c r="I2" t="s">
         <v>4</v>
       </c>
       <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1">
         <v>-14</v>
@@ -624,18 +645,21 @@
         <v>14</v>
       </c>
       <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1">
         <v>-14</v>
@@ -650,18 +674,21 @@
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1">
         <v>-14</v>
@@ -676,18 +703,21 @@
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -696,7 +726,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1">
         <v>10</v>
@@ -705,18 +735,21 @@
         <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1">
         <v>6478</v>
@@ -725,18 +758,21 @@
         <v>6378</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1">
         <v>6478</v>
@@ -745,18 +781,21 @@
         <v>6378</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1">
         <v>6478</v>
@@ -765,18 +804,21 @@
         <v>6378</v>
       </c>
       <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1">
         <v>6478</v>
@@ -785,18 +827,24 @@
         <v>6378</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
         <v>18</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="J11" t="s">
         <v>20</v>
       </c>
-      <c r="J11" t="s">
-        <v>21</v>
+      <c r="K11" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>